<commit_message>
Correction of errors in test cases
</commit_message>
<xml_diff>
--- a/Tests/Test Cases.xlsx
+++ b/Tests/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gato-\OneDrive\Рабочий стол\Новая папка\lab-grader\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F10953E-0977-42AA-B0B2-6D2B1862A1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EBC8AE-B1AC-4651-9D2A-E63602AAD951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6325525-B727-4748-9B35-D7788ECE9D16}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>id:</t>
   </si>
@@ -48,18 +48,9 @@
     <t>Проверка корректной работы функционала метода check_lab при валидных данных</t>
   </si>
   <si>
-    <t>1. Настроить программу lab-grader на работу с тестовой таблицой: https://docs.google.com/spreadsheets/d/17Qy4CFnqB3jKV9WC1TYzxQSlK-tolBmrW4Y8m1w2QXg/edit#gid=1593948738</t>
-  </si>
-  <si>
-    <t>2. После того как в пунке со статусом выполнения тестов на сайте: https://github.com/suai-ms-2020/ms-task1-BatMaxim появиться галочка, в консоли выполнения теста нажать любую клавишу для продолжения работы теста.</t>
-  </si>
-  <si>
     <t>Запуститься программа lab-grader</t>
   </si>
   <si>
-    <t>В ячейче соответствующей 1й лабораторной работе для студента Иванова Ивана Ивановича должа появиться галочка.</t>
-  </si>
-  <si>
     <t>Проверка корректной работы функционала метода check_lab при невалидном варианте работы</t>
   </si>
   <si>
@@ -75,13 +66,28 @@
     <t>1. Запустить файл Test2.bat</t>
   </si>
   <si>
-    <t>Из удаленного репозиторя студента будут удалены файлы проекта.</t>
-  </si>
-  <si>
     <t>3. После выполнения работы lab-grader в консоли выполнения теста нажать любую клавишу для продолжения работы теста.</t>
   </si>
   <si>
     <t>4. Перейти в таблицу: https://docs.google.com/spreadsheets/d/17Qy4CFnqB3jKV9WC1TYzxQSlK-tolBmrW4Y8m1w2QXg/edit#gid=1593948738</t>
+  </si>
+  <si>
+    <t>1. Настроить программу lab-grader на работу с тестовой таблицей: https://docs.google.com/spreadsheets/d/17Qy4CFnqB3jKV9WC1TYzxQSlK-tolBmrW4Y8m1w2QXg/edit#gid=1593948738</t>
+  </si>
+  <si>
+    <t>2. После того как в пункте со статусом выполнения тестов на сайте: https://github.com/suai-ms-2020/ms-task1-BatMaxim появиться галочка, в консоли выполнения теста нажать любую клавишу для продолжения работы теста.</t>
+  </si>
+  <si>
+    <t>В ячейке соответствующей 1й лабораторной работе для студента Иванова Ивана Ивановича должна появиться галочка.</t>
+  </si>
+  <si>
+    <t>Из удаленного репозитория студента будут удалены файлы проекта.</t>
+  </si>
+  <si>
+    <t>2. После того как в пунте со статусом выполнения тестов на сайте: https://github.com/suai-ms-2020/ms-task1-BatMaxim появиться галочка, в консоли выполнения теста нажать любую клавишу для продолжения работы теста.</t>
+  </si>
+  <si>
+    <t>В ячейке соответствующей 1й лабораторной работе для студента Иванова Ивана Ивановича должна появиться надпись, сообщающая о неправильном варианте.</t>
   </si>
 </sst>
 </file>
@@ -217,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -255,6 +261,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -264,18 +288,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,11 +297,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B8A38E-598F-4755-B154-02380F252339}">
   <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,19 +631,19 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:4" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -650,65 +659,65 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="2:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="22"/>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="2:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="B8" s="22"/>
+      <c r="C8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B9" s="23"/>
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16"/>
-      <c r="C7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
-      <c r="C9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="15">
         <v>2</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="2:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="21"/>
+      <c r="C12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="2:4" ht="18" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -724,56 +733,56 @@
         <v>4</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="108" x14ac:dyDescent="0.3">
+      <c r="B16" s="25"/>
+      <c r="C16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="108" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
-      <c r="C16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="17" spans="2:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="24"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="90" x14ac:dyDescent="0.3">
+      <c r="B18" s="26"/>
       <c r="C18" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>